<commit_message>
Added cadetes pages and functionalities
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESCRITORIO\TaxiMoto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC63480-B146-4D8C-9976-6577FC472DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD1C091-A6BE-48DF-AB66-78AC4BD08B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -612,7 +612,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
improved backend logic and user experience
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESCRITORIO\TaxiMoto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD1C091-A6BE-48DF-AB66-78AC4BD08B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C42E22A-A1E7-48A8-B441-07F90716FAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -612,7 +612,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="E2:F2"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding information to detail page
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESCRITORIO\TaxiMoto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C42E22A-A1E7-48A8-B441-07F90716FAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6252C963-EE16-4D7C-80A7-B2A5369DA15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3705" yWindow="1890" windowWidth="25080" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>3496-461432</t>
   </si>
@@ -246,6 +246,21 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>Wow coffee bar</t>
+  </si>
+  <si>
+    <t>Moreno 2201</t>
+  </si>
+  <si>
+    <t>[-31.447512460528124, -60.932169283415085]</t>
+  </si>
+  <si>
+    <t>wowcoffee</t>
+  </si>
+  <si>
+    <t>wowcoffee2201</t>
   </si>
 </sst>
 </file>
@@ -609,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E248A01-8996-694C-998D-284EA5AE4B47}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,11 +880,34 @@
         <v>67</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>